<commit_message>
Fixing Error with numbers in last name
</commit_message>
<xml_diff>
--- a/application/data/StudentData.xlsx
+++ b/application/data/StudentData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mecha\Documents\GitHub\Invited-Meeting-Scheduler\application\data\"/>
     </mc:Choice>
@@ -14,10 +14,11 @@
   </bookViews>
   <sheets>
     <sheet name="RawData" sheetId="1" r:id="rId1"/>
+    <sheet name="ScheduleData" r:id="rId5" sheetId="2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -47,11 +48,27 @@
   <si>
     <t>Humanities</t>
   </si>
+  <si>
+    <t>Rotations Needed</t>
+  </si>
+  <si>
+    <t>ROT1</t>
+  </si>
+  <si>
+    <t>ROT2</t>
+  </si>
+  <si>
+    <t>ROT3</t>
+  </si>
+  <si>
+    <t>ROT4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -389,7 +406,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1576,4 +1593,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>